<commit_message>
Cacheo de objetos desactivado en contenido
</commit_message>
<xml_diff>
--- a/Documentacion/Performance/TestDePerformanceMapeadorVortex.xlsx
+++ b/Documentacion/Performance/TestDePerformanceMapeadorVortex.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Test</t>
   </si>
@@ -36,10 +36,22 @@
     <t>modelo</t>
   </si>
   <si>
-    <t>Obj-&gt;Vortex</t>
-  </si>
-  <si>
     <t>Vortex-&gt;Obj</t>
+  </si>
+  <si>
+    <t>TestMapeoAVortex</t>
+  </si>
+  <si>
+    <t>Hola manola</t>
+  </si>
+  <si>
+    <t>(Obj/ms)</t>
+  </si>
+  <si>
+    <t>Obj-&gt;Vortex (obj/ms)</t>
+  </si>
+  <si>
+    <t>ClaseParaProbarMapeo</t>
   </si>
 </sst>
 </file>
@@ -378,16 +390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:E12"/>
+  <dimension ref="C4:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -399,56 +411,85 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>252.91470000000001</v>
+      </c>
+      <c r="E7">
+        <v>252.91460000000001</v>
+      </c>
+    </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>263.20710000000003</v>
+      </c>
+      <c r="E8">
+        <v>263.20699999999999</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>250.62909307402199</v>
+        <v>236.62889999999999</v>
       </c>
       <c r="E9">
-        <v>250.62899384798499</v>
+        <v>236.62880000000001</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>275.76830000000001</v>
+        <v>31.4053</v>
       </c>
       <c r="E10">
-        <v>275.76819999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>236.02610000000001</v>
-      </c>
-      <c r="E11">
-        <v>236.02610000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>368.38330000000002</v>
-      </c>
-      <c r="E12">
-        <v>368.38330000000002</v>
+        <v>31.4053</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>228.83295194508</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>1.0406585287169701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>